<commit_message>
Test openpyxl in case of sharing
</commit_message>
<xml_diff>
--- a/openpyxl/target.xlsx
+++ b/openpyxl/target.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-K70V6GV\TUTORIAL-excel-with-python\openpyxl\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B04F7A0-E6A6-41CE-8D86-ED5103A9D219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -53,7 +65,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +342,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>